<commit_message>
Added detail to the main description
</commit_message>
<xml_diff>
--- a/1D Euler/Speeding up Python.xlsx
+++ b/1D Euler/Speeding up Python.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pulsar/Documents/MSU/CA_CFD/1D Euler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905FDDC9-F90F-6C41-8DA8-0139BE400FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EA585E-62A9-1A41-8EBB-3AAB062D2F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{00ADC960-4800-E342-BCEB-7005C541E381}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Comments</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>cleaned up code after the last timing update (removing unnessary import statements, deleting commented out bits of code)</t>
+  </si>
+  <si>
+    <t>replacing L = np.linalg.inv(R) with the correct formula</t>
   </si>
 </sst>
 </file>
@@ -522,7 +525,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -621,9 +624,17 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="3">
+        <f>(7.9654+7.6745+7.82873)/3</f>
+        <v>7.8228766666666667</v>
+      </c>
+      <c r="B8" s="3">
+        <f>A8/60</f>
+        <v>0.13038127777777778</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>

</xml_diff>